<commit_message>
Add a working example data-sheet
</commit_message>
<xml_diff>
--- a/data/data_example.xlsx
+++ b/data/data_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lennard\Documents\MTS. de Ruijter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBB858E4-84A4-491F-827D-CF0AD264DBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{55883317-D1D4-480E-BFD1-FFE0450F0515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{34385EA3-E32E-46B3-8889-20CF654E67DA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Categorie</t>
   </si>
@@ -218,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -232,6 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD33EFF-5429-410E-939F-DC0D953F10E5}">
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -726,16 +727,16 @@
         <v>100</v>
       </c>
       <c r="I2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J2">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="K2" t="s">
         <v>25</v>
       </c>
       <c r="L2">
-        <v>360</v>
+        <v>380</v>
       </c>
       <c r="M2" t="s">
         <v>25</v>
@@ -747,16 +748,16 @@
         <v>70</v>
       </c>
       <c r="P2">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="Q2">
         <v>60</v>
       </c>
       <c r="R2">
-        <v>19</v>
-      </c>
-      <c r="S2">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>25</v>
       </c>
       <c r="T2" t="s">
         <v>25</v>
@@ -765,10 +766,12 @@
         <v>25</v>
       </c>
       <c r="V2">
-        <v>2</v>
+        <f>2/19</f>
+        <v>0.10526315789473684</v>
       </c>
       <c r="W2">
-        <v>2</v>
+        <f>2/19</f>
+        <v>0.10526315789473684</v>
       </c>
     </row>
     <row r="3" spans="1:24">
@@ -777,52 +780,55 @@
       </c>
       <c r="D3" s="5"/>
       <c r="F3" s="6">
-        <v>1000</v>
+        <v>950</v>
       </c>
       <c r="G3">
-        <v>508</v>
+        <v>550</v>
       </c>
       <c r="H3">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="Q3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="R3">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="S3">
-        <v>13.5</v>
+        <f>13/19</f>
+        <v>0.68421052631578949</v>
       </c>
       <c r="T3">
-        <v>4</v>
+        <f>4/19</f>
+        <v>0.21052631578947367</v>
       </c>
       <c r="U3">
-        <v>4</v>
+        <f>4/19</f>
+        <v>0.21052631578947367</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -892,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -964,7 +970,7 @@
         <v>0</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -1809,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="W18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X18" s="3"/>
     </row>
@@ -2022,7 +2028,9 @@
     </row>
     <row r="22" spans="2:24"/>
     <row r="23" spans="2:24"/>
-    <row r="24" spans="2:24"/>
+    <row r="24" spans="2:24">
+      <c r="B24" s="7"/>
+    </row>
     <row r="25" spans="2:24"/>
     <row r="26" spans="2:24"/>
     <row r="27" spans="2:24"/>

</xml_diff>